<commit_message>
SkyBox added Models/Textures Added Milky Way Created
</commit_message>
<xml_diff>
--- a/Project_Rubric.xlsx
+++ b/Project_Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -931,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1553,9 @@
       <c r="D23" s="5">
         <v>3</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
@@ -3048,7 +3053,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Update Milestone 3 - Directional, Point and Spot light working - Instantiating properly done - Input layout changed
</commit_message>
<xml_diff>
--- a/Project_Rubric.xlsx
+++ b/Project_Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,18 +1057,20 @@
       <c r="E4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G4" s="17">
         <f t="shared" ref="G4:G35" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1077,7 +1082,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1096,10 +1101,12 @@
       <c r="E5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1128,11 +1135,15 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 18,0)</f>
@@ -1204,11 +1215,11 @@
       </c>
       <c r="H8" s="19">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1429,10 +1440,12 @@
       <c r="E18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1556,10 +1569,12 @@
       <c r="E23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1695,10 +1710,12 @@
       <c r="E30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G30" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1722,10 +1739,12 @@
       <c r="E31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G31" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1749,10 +1768,12 @@
       <c r="E32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G32" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -2446,10 +2467,12 @@
       <c r="E65" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G65" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -2473,10 +2496,12 @@
       <c r="E66" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G66" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -3059,7 +3084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Click to check updates - Light rotation - Independent viewports - Independent cameras - Normal texture incremented - Transparency incremented
</commit_message>
<xml_diff>
--- a/Project_Rubric.xlsx
+++ b/Project_Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -374,6 +374,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>https://takinginitiative.wordpress.com/2010/07/30/directx-10-tutorial-7-viewports/</t>
+  </si>
+  <si>
+    <t>https://msdn.microsoft.com/en-us/library/windows/desktop/ee663274(v=vs.85).aspx</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -937,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,11 +1075,11 @@
       </c>
       <c r="H4" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1082,7 +1091,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1215,11 +1224,11 @@
       </c>
       <c r="H8" s="19">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1541,7 +1550,9 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
@@ -1944,7 +1955,9 @@
       <c r="D39" s="5">
         <v>2</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="17">
         <f t="shared" si="1"/>
@@ -2522,7 +2535,9 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="F67" s="3"/>
       <c r="G67" s="17">
         <f t="shared" si="1"/>
@@ -2547,7 +2562,9 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="G68" s="17">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -2931,8 +2948,12 @@
       <c r="B90" s="6">
         <v>2</v>
       </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -2994,10 +3015,14 @@
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
+      <c r="A95" s="13" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
+      <c r="A96" s="13" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>

</xml_diff>

<commit_message>
Update - GeometryShader - Specular Mapping
</commit_message>
<xml_diff>
--- a/Project_Rubric.xlsx
+++ b/Project_Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>https://github.com/Microsoft/HoloLensCompanionKit/tree/master/RemotingHostSample/RemotingHostSampleShared</t>
   </si>
 </sst>
 </file>
@@ -946,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1086,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1091,7 +1094,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1232,7 +1235,7 @@
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1553,10 +1556,12 @@
       <c r="E22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1830,11 +1835,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G34" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1855,11 +1864,15 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G35" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1958,10 +1971,12 @@
       <c r="E39" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G39" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2538,10 +2553,12 @@
       <c r="E67" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G67" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -2565,10 +2582,12 @@
       <c r="E68" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F68" s="3"/>
+      <c r="F68" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G68" s="17">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -2954,7 +2973,9 @@
       <c r="D90" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3025,7 +3046,9 @@
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="13"/>
+      <c r="A97" s="13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
@@ -3109,7 +3132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>